<commit_message>
style: increase font sizes across all pages for better readability and accessibility
</commit_message>
<xml_diff>
--- a/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
+++ b/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC5F4B2-E44E-45DE-B45A-808B9BC8AF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058BA82D-CFBA-40C8-9160-69D62609C4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E40E823-4079-41FB-B2B7-348FD665EC3B}"/>
   </bookViews>
@@ -307,71 +307,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -690,16 +690,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D026C704-A60F-436A-8943-420E91A4FB12}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="13" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -721,88 +721,88 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>4</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -816,62 +816,62 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="21">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="15" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="21">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>7</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -883,45 +883,45 @@
       <c r="E13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="18"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="21">
+        <v>8</v>
+      </c>
+      <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="23" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="24"/>
     </row>
     <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="A16" s="25">
         <v>9</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="18" t="s">
         <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -929,34 +929,34 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22">
+      <c r="A19" s="9">
         <v>10</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="15" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="18" t="s">
         <v>43</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -965,25 +965,25 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="17"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -998,7 +998,7 @@
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1012,8 +1012,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24" t="s">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1025,7 +1025,7 @@
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
         <v>55</v>
@@ -1043,18 +1043,21 @@
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
+      <c r="A27" s="10"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
@@ -1067,14 +1070,11 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: update coordination list and add trial scripts
</commit_message>
<xml_diff>
--- a/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
+++ b/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058BA82D-CFBA-40C8-9160-69D62609C4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070AC5CA-877D-489F-B3F0-64F102EC44FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E40E823-4079-41FB-B2B7-348FD665EC3B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>No</t>
   </si>
@@ -196,13 +196,52 @@
   </si>
   <si>
     <t>XII.3</t>
+  </si>
+  <si>
+    <t>Taufik Hidayat, S.Pd.</t>
+  </si>
+  <si>
+    <t>XII.4</t>
+  </si>
+  <si>
+    <t>XII.5</t>
+  </si>
+  <si>
+    <t>XII.6</t>
+  </si>
+  <si>
+    <t>koor_taufik</t>
+  </si>
+  <si>
+    <t>Mas’ud abid, S.Pd., M.Pd.</t>
+  </si>
+  <si>
+    <t>XII.7</t>
+  </si>
+  <si>
+    <t>XII.8</t>
+  </si>
+  <si>
+    <t>koor_abid</t>
+  </si>
+  <si>
+    <t>Ade Rohmah Apriani, S.Pd.</t>
+  </si>
+  <si>
+    <t>XII.9</t>
+  </si>
+  <si>
+    <t>XII.10</t>
+  </si>
+  <si>
+    <t>koor_ade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,6 +260,12 @@
       <color rgb="FF0A0A0A"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,35 +342,10 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -344,35 +364,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,35 +733,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D026C704-A60F-436A-8943-420E91A4FB12}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -724,51 +769,51 @@
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="3" t="s">
+      <c r="E2" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="24"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="3" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="25"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="A5" s="19">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -776,42 +821,42 @@
       <c r="A6" s="21">
         <v>3</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+      <c r="A8" s="19">
         <v>4</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="10" t="s">
         <v>8</v>
       </c>
     </row>
@@ -819,245 +864,346 @@
       <c r="A9" s="21">
         <v>5</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="3" t="s">
+      <c r="E9" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <v>6</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="3" t="s">
+      <c r="E11" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="24"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="A13" s="19">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="8"/>
+      <c r="E13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <v>8</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="3" t="s">
+      <c r="E14" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="24"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+      <c r="A16" s="23">
         <v>9</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="3" t="s">
+      <c r="E16" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="3" t="s">
+      <c r="D17" s="22"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="21">
         <v>10</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="3" t="s">
+      <c r="E19" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="24"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="3" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="10"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="25"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="27">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="19">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+      <c r="E23" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>13</v>
+      </c>
       <c r="B24" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3" t="s">
+      <c r="E24" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3" t="s">
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>14</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>16</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="16"/>
+      <c r="E33" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
+  <mergeCells count="40">
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A19:A21"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
@@ -1070,12 +1216,16 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: implement monitoring, participation stats, and detailed analysis in coordinator dashboard
</commit_message>
<xml_diff>
--- a/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
+++ b/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070AC5CA-877D-489F-B3F0-64F102EC44FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A8DB53-FB4E-4A1E-8DE0-D208D1F38EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E40E823-4079-41FB-B2B7-348FD665EC3B}"/>
   </bookViews>
@@ -241,7 +241,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +263,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,10 +352,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -419,8 +435,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -735,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D026C704-A60F-436A-8943-420E91A4FB12}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,19 +776,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
@@ -778,7 +805,7 @@
       <c r="D2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1226,6 +1253,9 @@
     <mergeCell ref="E6:E7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D2EBBF4C-5269-47C8-A18C-52C69E2498AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: implement facilitator dashboard, register 60 facilitator accounts and 1 admin account
</commit_message>
<xml_diff>
--- a/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
+++ b/DAFTAR KOORDINATOR DAN FASILITAOTOR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aplikasi Web AI\LP Kokulikuler SMAN 1 Belitang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A8DB53-FB4E-4A1E-8DE0-D208D1F38EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8BF0E4-F2CD-4245-AD70-8E6A84865609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E40E823-4079-41FB-B2B7-348FD665EC3B}"/>
   </bookViews>
@@ -356,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -371,79 +371,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -763,7 +766,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,33 +779,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="31" t="s">
@@ -810,427 +813,415 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="24"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="10" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="32" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="22" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="10" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="25"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+      <c r="A8" s="7">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9" s="22">
         <v>5</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="29"/>
     </row>
     <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="22">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="10" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="16"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="7">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
-        <v>8</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="22">
+        <v>8</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="27" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
+      <c r="A16" s="29">
         <v>9</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10" t="s">
+      <c r="A17" s="29"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="29"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+      <c r="A19" s="22">
         <v>10</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="27">
+      <c r="A22" s="10">
         <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="A23" s="7">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
+      <c r="A24" s="17">
         <v>13</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="10" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="10" t="s">
+      <c r="A26" s="19"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
+      <c r="A27" s="17">
         <v>14</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="17" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="10" t="s">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="10" t="s">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
+      <c r="A30" s="17">
         <v>15</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="10" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="A32" s="17">
         <v>16</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="10" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="10"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="B16:B18"/>
@@ -1243,18 +1234,31 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="E11:E12"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{D2EBBF4C-5269-47C8-A18C-52C69E2498AD}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{DE1D54B4-A956-4329-8D13-FCCAF68010B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>